<commit_message>
Corrected ERP to output in a more R-friendly style. Completed R analysis of ERP components. Still trying to get FFT correct for Freq analysis, currently focusing on JUST the gamma band from the original paper...
</commit_message>
<xml_diff>
--- a/Stats/Statistics.xlsx
+++ b/Stats/Statistics.xlsx
@@ -8,21 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\PycharmProjects\Pain\Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B107A38-87DB-4F06-B879-1D47236DF0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FB56EB-7EEC-4409-9B06-BDCBF3EF9151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{30898942-D181-4398-8C06-282691AD810A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{30898942-D181-4398-8C06-282691AD810A}"/>
   </bookViews>
   <sheets>
     <sheet name="Gender &amp; Pain Threshold" sheetId="1" r:id="rId1"/>
     <sheet name="Gender &amp; Pain Rating" sheetId="2" r:id="rId2"/>
-    <sheet name="ERP Grouped" sheetId="4" r:id="rId3"/>
-    <sheet name="ERP by Subject" sheetId="5" r:id="rId4"/>
+    <sheet name="ERP Components" sheetId="5" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId5"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'ERP by Subject'!$A$1:$T$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'ERP Components'!$A$1:$T$53</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Gender &amp; Pain Rating'!$A$1:$D$3061</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Gender &amp; Pain Threshold'!$C$1:$D$52</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">'Gender &amp; Pain Threshold'!$F$1</definedName>
@@ -51,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6335" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6349" uniqueCount="58">
   <si>
     <t>Subject</t>
   </si>
@@ -296,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -306,42 +302,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -388,14 +362,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Gender Differences in PREP</a:t>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Gender Differences in PREP Latencies</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Latencies</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -440,7 +414,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ERP Grouped'!$A$3</c:f>
+              <c:f>'ERP Components'!$V$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -459,9 +433,27 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'ERP Grouped'!$B$1:$G$2</c:f>
+              <c:f>'ERP Components'!$W$2:$AB$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="6"/>
                 <c:lvl>
@@ -497,34 +489,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ERP Grouped'!$B$3:$G$3</c:f>
+              <c:f>'ERP Components'!$W$4:$AB$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>160</c:v>
+                  <c:v>162.82978723404256</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156</c:v>
+                  <c:v>162.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>152</c:v>
+                  <c:v>161.88</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>152</c:v>
+                  <c:v>162.82978723404256</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>164</c:v>
+                  <c:v>162.52000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>152</c:v>
+                  <c:v>161.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8366-4048-9A59-43451F99D41B}"/>
+              <c16:uniqueId val="{00000000-621C-4331-BBBC-A3475B1EAB89}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -533,7 +525,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ERP Grouped'!$A$4</c:f>
+              <c:f>'ERP Components'!$V$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -552,9 +544,27 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'ERP Grouped'!$B$1:$G$2</c:f>
+              <c:f>'ERP Components'!$W$2:$AB$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="6"/>
                 <c:lvl>
@@ -590,34 +600,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ERP Grouped'!$B$4:$G$4</c:f>
+              <c:f>'ERP Components'!$W$5:$AB$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>196</c:v>
+                  <c:v>193.16666666666666</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>196</c:v>
+                  <c:v>191.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>196</c:v>
+                  <c:v>190.91836734693877</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>184</c:v>
+                  <c:v>193</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>184</c:v>
+                  <c:v>191.24489795918367</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>180</c:v>
+                  <c:v>190.83673469387756</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8366-4048-9A59-43451F99D41B}"/>
+              <c16:uniqueId val="{00000001-621C-4331-BBBC-A3475B1EAB89}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -626,7 +636,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ERP Grouped'!$A$5</c:f>
+              <c:f>'ERP Components'!$V$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -645,9 +655,27 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'ERP Grouped'!$B$1:$G$2</c:f>
+              <c:f>'ERP Components'!$W$2:$AB$3</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="6"/>
                 <c:lvl>
@@ -683,34 +711,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ERP Grouped'!$B$5:$G$5</c:f>
+              <c:f>'ERP Components'!$W$6:$AB$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>316</c:v>
+                  <c:v>306.48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>320</c:v>
+                  <c:v>308.25531914893617</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>320</c:v>
+                  <c:v>309.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>292</c:v>
+                  <c:v>306.39999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>292</c:v>
+                  <c:v>307.65957446808511</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>300</c:v>
+                  <c:v>309.08333333333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-8366-4048-9A59-43451F99D41B}"/>
+              <c16:uniqueId val="{00000002-621C-4331-BBBC-A3475B1EAB89}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -724,11 +752,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1435550575"/>
-        <c:axId val="1435550991"/>
+        <c:axId val="666593919"/>
+        <c:axId val="666602655"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1435550575"/>
+        <c:axId val="666593919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -771,7 +799,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1435550991"/>
+        <c:crossAx val="666602655"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -779,7 +807,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1435550991"/>
+        <c:axId val="666602655"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +858,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1435550575"/>
+        <c:crossAx val="666593919"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -944,9 +972,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
               <a:t>Gender Differences in PREP Amplitudes</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -991,7 +1024,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ERP Grouped'!$A$12</c:f>
+              <c:f>'ERP Components'!$V$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1010,9 +1043,27 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'ERP Grouped'!$B$10:$G$11</c:f>
+              <c:f>'ERP Components'!$W$11:$AB$12</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="6"/>
                 <c:lvl>
@@ -1048,34 +1099,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ERP Grouped'!$B$12:$G$12</c:f>
+              <c:f>'ERP Components'!$W$13:$AB$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.8540000000000001</c:v>
+                  <c:v>3.2930496839562009</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0599999999999996</c:v>
+                  <c:v>3.5469417233629263</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.9380000000000002</c:v>
+                  <c:v>3.3347560546044916</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.331</c:v>
+                  <c:v>3.2075163709420136</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.363</c:v>
+                  <c:v>3.5081309982243818</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0139999999999998</c:v>
+                  <c:v>3.2695513116452446</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5E85-47BE-AE47-E61E0B46978F}"/>
+              <c16:uniqueId val="{00000000-87EC-422E-B03A-C9527AB462D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1084,7 +1135,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ERP Grouped'!$A$13</c:f>
+              <c:f>'ERP Components'!$V$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1103,9 +1154,27 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'ERP Grouped'!$B$10:$G$11</c:f>
+              <c:f>'ERP Components'!$W$11:$AB$12</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="6"/>
                 <c:lvl>
@@ -1141,34 +1210,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ERP Grouped'!$B$13:$G$13</c:f>
+              <c:f>'ERP Components'!$W$14:$AB$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.76</c:v>
+                  <c:v>5.1427575286769924</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.4450000000000003</c:v>
+                  <c:v>5.9068372801446598</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.9020000000000001</c:v>
+                  <c:v>6.2242932365196042</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.7559999999999998</c:v>
+                  <c:v>5.0223362594355825</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.6989999999999998</c:v>
+                  <c:v>5.8757264681742249</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8029999999999999</c:v>
+                  <c:v>6.1901875622429543</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5E85-47BE-AE47-E61E0B46978F}"/>
+              <c16:uniqueId val="{00000001-87EC-422E-B03A-C9527AB462D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1177,7 +1246,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'ERP Grouped'!$A$14</c:f>
+              <c:f>'ERP Components'!$V$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1196,9 +1265,27 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'ERP Grouped'!$B$10:$G$11</c:f>
+              <c:f>'ERP Components'!$W$11:$AB$12</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="6"/>
                 <c:lvl>
@@ -1234,34 +1321,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'ERP Grouped'!$B$14:$G$14</c:f>
+              <c:f>'ERP Components'!$W$15:$AB$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.8049999999999997</c:v>
+                  <c:v>4.0215520904838993</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8819999999999997</c:v>
+                  <c:v>5.0644995937052171</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.742</c:v>
+                  <c:v>5.9437972947243018</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.073</c:v>
+                  <c:v>3.911610406559431</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3319999999999999</c:v>
+                  <c:v>5.0510473583514113</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.56</c:v>
+                  <c:v>5.9394200998251057</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-5E85-47BE-AE47-E61E0B46978F}"/>
+              <c16:uniqueId val="{00000002-87EC-422E-B03A-C9527AB462D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1275,11 +1362,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1526114703"/>
-        <c:axId val="1526128015"/>
+        <c:axId val="663947807"/>
+        <c:axId val="663948223"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1526114703"/>
+        <c:axId val="663947807"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1322,7 +1409,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1526128015"/>
+        <c:crossAx val="663948223"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1330,7 +1417,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1526128015"/>
+        <c:axId val="663948223"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1381,7 +1468,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1526114703"/>
+        <c:crossAx val="663947807"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3244,8 +3331,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7686675" y="2835592"/>
-              <a:ext cx="5265420" cy="4125278"/>
+              <a:off x="7684770" y="2810827"/>
+              <a:ext cx="5248275" cy="4090988"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3282,29 +3369,27 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>478155</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{036FA315-D509-455B-BCCE-FD1D0EC8F004}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90B596D9-49C7-E0A0-DD36-044AC5D083A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3320,29 +3405,27 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>521970</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>167640</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>80010</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69D2DAEA-1C88-430C-A3FA-0600739972A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECCA102E-9573-76B7-176B-19130D2424FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3357,216 +3440,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Grouped"/>
-      <sheetName val="Seperated"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>Male</v>
-          </cell>
-          <cell r="E1" t="str">
-            <v>Female</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>Low</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>Med</v>
-          </cell>
-          <cell r="D2" t="str">
-            <v>High</v>
-          </cell>
-          <cell r="E2" t="str">
-            <v>Low</v>
-          </cell>
-          <cell r="F2" t="str">
-            <v>Med</v>
-          </cell>
-          <cell r="G2" t="str">
-            <v>High</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>N1 Lat</v>
-          </cell>
-          <cell r="B3">
-            <v>160</v>
-          </cell>
-          <cell r="C3">
-            <v>156</v>
-          </cell>
-          <cell r="D3">
-            <v>152</v>
-          </cell>
-          <cell r="E3">
-            <v>152</v>
-          </cell>
-          <cell r="F3">
-            <v>164</v>
-          </cell>
-          <cell r="G3">
-            <v>152</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>N2 Lat</v>
-          </cell>
-          <cell r="B4">
-            <v>196</v>
-          </cell>
-          <cell r="C4">
-            <v>196</v>
-          </cell>
-          <cell r="D4">
-            <v>196</v>
-          </cell>
-          <cell r="E4">
-            <v>184</v>
-          </cell>
-          <cell r="F4">
-            <v>184</v>
-          </cell>
-          <cell r="G4">
-            <v>180</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>P2 Lat</v>
-          </cell>
-          <cell r="B5">
-            <v>316</v>
-          </cell>
-          <cell r="C5">
-            <v>320</v>
-          </cell>
-          <cell r="D5">
-            <v>320</v>
-          </cell>
-          <cell r="E5">
-            <v>292</v>
-          </cell>
-          <cell r="F5">
-            <v>292</v>
-          </cell>
-          <cell r="G5">
-            <v>300</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>Male</v>
-          </cell>
-          <cell r="E10" t="str">
-            <v>Female</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v>Low</v>
-          </cell>
-          <cell r="C11" t="str">
-            <v>Med</v>
-          </cell>
-          <cell r="D11" t="str">
-            <v>High</v>
-          </cell>
-          <cell r="E11" t="str">
-            <v>Low</v>
-          </cell>
-          <cell r="F11" t="str">
-            <v>Med</v>
-          </cell>
-          <cell r="G11" t="str">
-            <v>High</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>N1 Amp</v>
-          </cell>
-          <cell r="B12">
-            <v>3.8540000000000001</v>
-          </cell>
-          <cell r="C12">
-            <v>4.0599999999999996</v>
-          </cell>
-          <cell r="D12">
-            <v>3.9380000000000002</v>
-          </cell>
-          <cell r="E12">
-            <v>2.331</v>
-          </cell>
-          <cell r="F12">
-            <v>3.363</v>
-          </cell>
-          <cell r="G12">
-            <v>3.0139999999999998</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>N2 Amp</v>
-          </cell>
-          <cell r="B13">
-            <v>5.76</v>
-          </cell>
-          <cell r="C13">
-            <v>6.4450000000000003</v>
-          </cell>
-          <cell r="D13">
-            <v>6.9020000000000001</v>
-          </cell>
-          <cell r="E13">
-            <v>3.7559999999999998</v>
-          </cell>
-          <cell r="F13">
-            <v>4.6989999999999998</v>
-          </cell>
-          <cell r="G13">
-            <v>4.8029999999999999</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>P2 Amp</v>
-          </cell>
-          <cell r="B14">
-            <v>4.8049999999999997</v>
-          </cell>
-          <cell r="C14">
-            <v>4.8819999999999997</v>
-          </cell>
-          <cell r="D14">
-            <v>5.742</v>
-          </cell>
-          <cell r="E14">
-            <v>3.073</v>
-          </cell>
-          <cell r="F14">
-            <v>4.3319999999999999</v>
-          </cell>
-          <cell r="G14">
-            <v>5.56</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -84482,407 +84355,149 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACAACE5-BB1B-4726-AC1A-D5CAE172C067}">
-  <dimension ref="A1:G14"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3">
-        <v>160</v>
-      </c>
-      <c r="C3">
-        <v>156</v>
-      </c>
-      <c r="D3">
-        <v>152</v>
-      </c>
-      <c r="E3">
-        <v>152</v>
-      </c>
-      <c r="F3">
-        <v>164</v>
-      </c>
-      <c r="G3">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4">
-        <v>196</v>
-      </c>
-      <c r="C4">
-        <v>196</v>
-      </c>
-      <c r="D4">
-        <v>196</v>
-      </c>
-      <c r="E4">
-        <v>184</v>
-      </c>
-      <c r="F4">
-        <v>184</v>
-      </c>
-      <c r="G4">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5">
-        <v>316</v>
-      </c>
-      <c r="C5">
-        <v>320</v>
-      </c>
-      <c r="D5">
-        <v>320</v>
-      </c>
-      <c r="E5">
-        <v>292</v>
-      </c>
-      <c r="F5">
-        <v>292</v>
-      </c>
-      <c r="G5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6">
-        <v>-3.8540000000000001</v>
-      </c>
-      <c r="C6">
-        <v>-4.0599999999999996</v>
-      </c>
-      <c r="D6">
-        <v>-3.9380000000000002</v>
-      </c>
-      <c r="E6">
-        <v>-2.331</v>
-      </c>
-      <c r="F6">
-        <v>-3.363</v>
-      </c>
-      <c r="G6">
-        <v>-3.0139999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7">
-        <v>-5.76</v>
-      </c>
-      <c r="C7">
-        <v>-6.4450000000000003</v>
-      </c>
-      <c r="D7">
-        <v>-6.9020000000000001</v>
-      </c>
-      <c r="E7">
-        <v>-3.7559999999999998</v>
-      </c>
-      <c r="F7">
-        <v>-4.6989999999999998</v>
-      </c>
-      <c r="G7">
-        <v>-4.8029999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8">
-        <v>4.8049999999999997</v>
-      </c>
-      <c r="C8">
-        <v>4.8819999999999997</v>
-      </c>
-      <c r="D8">
-        <v>5.742</v>
-      </c>
-      <c r="E8">
-        <v>3.073</v>
-      </c>
-      <c r="F8">
-        <v>4.3319999999999999</v>
-      </c>
-      <c r="G8">
-        <v>5.56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12">
-        <v>3.8540000000000001</v>
-      </c>
-      <c r="C12">
-        <v>4.0599999999999996</v>
-      </c>
-      <c r="D12">
-        <v>3.9380000000000002</v>
-      </c>
-      <c r="E12">
-        <v>2.331</v>
-      </c>
-      <c r="F12">
-        <v>3.363</v>
-      </c>
-      <c r="G12">
-        <v>3.0139999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13">
-        <v>5.76</v>
-      </c>
-      <c r="C13">
-        <v>6.4450000000000003</v>
-      </c>
-      <c r="D13">
-        <v>6.9020000000000001</v>
-      </c>
-      <c r="E13">
-        <v>3.7559999999999998</v>
-      </c>
-      <c r="F13">
-        <v>4.6989999999999998</v>
-      </c>
-      <c r="G13">
-        <v>4.8029999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14">
-        <v>4.8049999999999997</v>
-      </c>
-      <c r="C14">
-        <v>4.8819999999999997</v>
-      </c>
-      <c r="D14">
-        <v>5.742</v>
-      </c>
-      <c r="E14">
-        <v>3.073</v>
-      </c>
-      <c r="F14">
-        <v>4.3319999999999999</v>
-      </c>
-      <c r="G14">
-        <v>5.56</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401EBBD2-3936-4E70-BEF6-9C13203BA8BC}">
   <dimension ref="A1:AB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="D1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="I1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="J1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="O1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
+      <c r="P1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="8" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="5" t="s">
         <v>56</v>
       </c>
+      <c r="W2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -84945,6 +84560,24 @@
       <c r="T3">
         <v>3.2223065475467898</v>
       </c>
+      <c r="W3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -85007,6 +84640,33 @@
       <c r="T4">
         <v>4.7981229402688399</v>
       </c>
+      <c r="V4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="W4" s="6">
+        <f>AVERAGE(C4:C53)</f>
+        <v>162.82978723404256</v>
+      </c>
+      <c r="X4" s="6">
+        <f>AVERAGE(I4:I53)</f>
+        <v>162.19999999999999</v>
+      </c>
+      <c r="Y4" s="6">
+        <f>AVERAGE(O4:O53)</f>
+        <v>161.88</v>
+      </c>
+      <c r="Z4" s="6">
+        <f>AVERAGE(C3:C52)</f>
+        <v>162.82978723404256</v>
+      </c>
+      <c r="AA4" s="6">
+        <f>AVERAGE(I3:I52)</f>
+        <v>162.52000000000001</v>
+      </c>
+      <c r="AB4" s="6">
+        <f>AVERAGE(O3:O52)</f>
+        <v>161.88</v>
+      </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -85069,6 +84729,33 @@
       <c r="T5">
         <v>1.0943922383659499</v>
       </c>
+      <c r="V5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="W5" s="6">
+        <f>AVERAGE(E4:E53)</f>
+        <v>193.16666666666666</v>
+      </c>
+      <c r="X5" s="6">
+        <f>AVERAGE(K3:K53)</f>
+        <v>191.08</v>
+      </c>
+      <c r="Y5" s="6">
+        <f>AVERAGE(Q4:Q53)</f>
+        <v>190.91836734693877</v>
+      </c>
+      <c r="Z5" s="6">
+        <f>AVERAGE(E3:E52)</f>
+        <v>193</v>
+      </c>
+      <c r="AA5" s="6">
+        <f>AVERAGE(K3:K52)</f>
+        <v>191.24489795918367</v>
+      </c>
+      <c r="AB5" s="6">
+        <f>AVERAGE(Q3:Q52)</f>
+        <v>190.83673469387756</v>
+      </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -85131,6 +84818,33 @@
       <c r="T6">
         <v>10.8856887637347</v>
       </c>
+      <c r="V6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="W6" s="6">
+        <f>AVERAGE(G4:G53)</f>
+        <v>306.48</v>
+      </c>
+      <c r="X6" s="6">
+        <f>AVERAGE(M4:M53)</f>
+        <v>308.25531914893617</v>
+      </c>
+      <c r="Y6" s="6">
+        <f>AVERAGE(S4:S53)</f>
+        <v>309.25</v>
+      </c>
+      <c r="Z6" s="6">
+        <f>AVERAGE(G3:G52)</f>
+        <v>306.39999999999998</v>
+      </c>
+      <c r="AA6" s="6">
+        <f>AVERAGE(M3:M52)</f>
+        <v>307.65957446808511</v>
+      </c>
+      <c r="AB6" s="6">
+        <f>AVERAGE(S3:S52)</f>
+        <v>309.08333333333331</v>
+      </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -85193,6 +84907,33 @@
       <c r="T7">
         <v>0.115858851408456</v>
       </c>
+      <c r="V7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="W7" s="6">
+        <f>AVERAGE(D4:D53)</f>
+        <v>-3.2930496839562009</v>
+      </c>
+      <c r="X7" s="6">
+        <f>AVERAGE(J4:J53)</f>
+        <v>-3.5469417233629263</v>
+      </c>
+      <c r="Y7" s="6">
+        <f>AVERAGE(P4:P53)</f>
+        <v>-3.3347560546044916</v>
+      </c>
+      <c r="Z7" s="6">
+        <f>AVERAGE(D3:D52)</f>
+        <v>-3.2075163709420136</v>
+      </c>
+      <c r="AA7" s="6">
+        <f>AVERAGE(J3:J52)</f>
+        <v>-3.5081309982243818</v>
+      </c>
+      <c r="AB7" s="6">
+        <f>AVERAGE(P3:P52)</f>
+        <v>-3.2695513116452446</v>
+      </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -85255,6 +84996,33 @@
       <c r="T8">
         <v>6.9938957784575102</v>
       </c>
+      <c r="V8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="W8" s="6">
+        <f>AVERAGE(F4:F53)</f>
+        <v>-5.1427575286769924</v>
+      </c>
+      <c r="X8" s="6">
+        <f>AVERAGE(L4:L53)</f>
+        <v>-5.9068372801446598</v>
+      </c>
+      <c r="Y8" s="6">
+        <f>AVERAGE(R4:R53)</f>
+        <v>-6.2242932365196042</v>
+      </c>
+      <c r="Z8" s="6">
+        <f>AVERAGE(F3:F52)</f>
+        <v>-5.0223362594355825</v>
+      </c>
+      <c r="AA8" s="6">
+        <f>AVERAGE(L3:L52)</f>
+        <v>-5.8757264681742249</v>
+      </c>
+      <c r="AB8" s="6">
+        <f>AVERAGE(R3:R52)</f>
+        <v>-6.1901875622429543</v>
+      </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -85317,6 +85085,33 @@
       <c r="T9">
         <v>3.47163934366549</v>
       </c>
+      <c r="V9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="W9" s="6">
+        <f>AVERAGE(H4:H53)</f>
+        <v>4.0215520904838993</v>
+      </c>
+      <c r="X9" s="6">
+        <f>AVERAGE(N4:N53)</f>
+        <v>5.0644995937052171</v>
+      </c>
+      <c r="Y9" s="6">
+        <f>AVERAGE(T4:T53)</f>
+        <v>5.9437972947243018</v>
+      </c>
+      <c r="Z9" s="6">
+        <f>AVERAGE(H3:H52)</f>
+        <v>3.911610406559431</v>
+      </c>
+      <c r="AA9" s="6">
+        <f>AVERAGE(N3:N52)</f>
+        <v>5.0510473583514113</v>
+      </c>
+      <c r="AB9" s="6">
+        <f>AVERAGE(T3:T52)</f>
+        <v>5.9394200998251057</v>
+      </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -85441,6 +85236,16 @@
       <c r="T11">
         <v>9.7466077591197102</v>
       </c>
+      <c r="W11" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -85503,6 +85308,24 @@
       <c r="T12">
         <v>3.6441446255961698</v>
       </c>
+      <c r="W12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="X12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z12" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB12" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -85565,6 +85388,33 @@
       <c r="T13">
         <v>6.7129603161284699</v>
       </c>
+      <c r="V13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="W13">
+        <f>ABS(W7)</f>
+        <v>3.2930496839562009</v>
+      </c>
+      <c r="X13">
+        <f t="shared" ref="X13:AB13" si="0">ABS(X7)</f>
+        <v>3.5469417233629263</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="0"/>
+        <v>3.3347560546044916</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="0"/>
+        <v>3.2075163709420136</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="0"/>
+        <v>3.5081309982243818</v>
+      </c>
+      <c r="AB13">
+        <f t="shared" si="0"/>
+        <v>3.2695513116452446</v>
+      </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -85627,6 +85477,33 @@
       <c r="T14">
         <v>5.8896439321202196</v>
       </c>
+      <c r="V14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="W14">
+        <f t="shared" ref="W14:AB14" si="1">ABS(W8)</f>
+        <v>5.1427575286769924</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="1"/>
+        <v>5.9068372801446598</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="1"/>
+        <v>6.2242932365196042</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="1"/>
+        <v>5.0223362594355825</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="1"/>
+        <v>5.8757264681742249</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="1"/>
+        <v>6.1901875622429543</v>
+      </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -85688,6 +85565,33 @@
       </c>
       <c r="T15">
         <v>6.9407784065449603</v>
+      </c>
+      <c r="V15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="W15">
+        <f t="shared" ref="W15:AB15" si="2">ABS(W9)</f>
+        <v>4.0215520904838993</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="2"/>
+        <v>5.0644995937052171</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="2"/>
+        <v>5.9437972947243018</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="2"/>
+        <v>3.911610406559431</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="2"/>
+        <v>5.0510473583514113</v>
+      </c>
+      <c r="AB15">
+        <f t="shared" si="2"/>
+        <v>5.9394200998251057</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
@@ -88064,15 +87968,16 @@
     <filterColumn colId="17" showButton="0"/>
     <filterColumn colId="18" showButton="0"/>
   </autoFilter>
-  <mergeCells count="7">
-    <mergeCell ref="Z1:AB1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="O1:T1"/>
+  <mergeCells count="6">
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="W11:Y11"/>
+    <mergeCell ref="Z11:AB11"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="W2:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>